<commit_message>
Add Male / Female section in student registration
</commit_message>
<xml_diff>
--- a/Campus2caretaker/Template/StudentRegistrationSample.xlsx
+++ b/Campus2caretaker/Template/StudentRegistrationSample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>StudentName</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>StudentAddress</t>
+  </si>
+  <si>
+    <t>Gender</t>
   </si>
 </sst>
 </file>
@@ -388,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,7 +410,7 @@
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -440,6 +443,9 @@
       </c>
       <c r="K1" t="s">
         <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Immediate notification to parents registered mobile number and registered email with password, when institute uploads student data for the first time.
</commit_message>
<xml_diff>
--- a/Campus2caretaker/Template/StudentRegistrationSample.xlsx
+++ b/Campus2caretaker/Template/StudentRegistrationSample.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>StudentName</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Gender</t>
+  </si>
+  <si>
+    <t>ParentsEmail</t>
   </si>
 </sst>
 </file>
@@ -391,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,7 +413,7 @@
     <col min="11" max="11" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -446,6 +449,9 @@
       </c>
       <c r="L1" t="s">
         <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>